<commit_message>
Finalized BOM v4 LED
Finalized BOM v4 with LEDS by:
- Fixing links
- Updating costs
- Overhauling formatting
</commit_message>
<xml_diff>
--- a/Documentation/Specifications Scratch Pad.xlsx
+++ b/Documentation/Specifications Scratch Pad.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noahm\Documents\GitHub\WilsonThrust510\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d7a43267b7fa0998/Github Repositories/WilsonThrust510/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76843577-0A13-4915-A722-162779F6504E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{76843577-0A13-4915-A722-162779F6504E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E95C89BB-93B8-438F-AE80-BC5B09B630D2}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="2" xr2:uid="{05D747D7-67EB-465A-918B-6E7BCC91F9F4}"/>
+    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{05D747D7-67EB-465A-918B-6E7BCC91F9F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Digikey" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="104">
   <si>
     <t>Operating Temperature</t>
   </si>
@@ -262,119 +262,101 @@
     <t>74HC165</t>
   </si>
   <si>
-    <t>Thread Pitch</t>
-  </si>
-  <si>
-    <t>Length</t>
-  </si>
-  <si>
-    <t>Threading</t>
-  </si>
-  <si>
-    <t>Fully Threaded</t>
-  </si>
-  <si>
-    <t>Head Diameter</t>
-  </si>
-  <si>
-    <t>Head Height</t>
-  </si>
-  <si>
-    <t>Countersink Angle</t>
-  </si>
-  <si>
-    <t>90°</t>
-  </si>
-  <si>
     <t>Drive Style</t>
   </si>
   <si>
-    <t>Drive Size</t>
-  </si>
-  <si>
-    <t>Material</t>
-  </si>
-  <si>
-    <t>Zinc-Plated Steel</t>
-  </si>
-  <si>
-    <t>Hardness</t>
-  </si>
-  <si>
-    <t>Rockwell B71</t>
-  </si>
-  <si>
-    <t>Tensile Strength</t>
-  </si>
-  <si>
-    <t>60,000 psi</t>
-  </si>
-  <si>
-    <t>Thread Type</t>
-  </si>
-  <si>
     <t>Metric</t>
   </si>
   <si>
-    <t>Thread Spacing</t>
-  </si>
-  <si>
     <t>Coarse</t>
   </si>
   <si>
-    <t>Thread Fit</t>
-  </si>
-  <si>
-    <t>Thread Direction</t>
-  </si>
-  <si>
     <t>Right Hand</t>
   </si>
   <si>
-    <t>Head Type</t>
-  </si>
-  <si>
-    <t>Flat</t>
-  </si>
-  <si>
-    <t>Flat Head Profile</t>
-  </si>
-  <si>
     <t>Standard</t>
   </si>
   <si>
-    <t>Thread Size</t>
-  </si>
-  <si>
     <t>M5</t>
   </si>
   <si>
     <t>0.8 mm</t>
   </si>
   <si>
-    <t>20 mm</t>
-  </si>
-  <si>
-    <t>9.2 mm</t>
-  </si>
-  <si>
-    <t>2.5 mm</t>
-  </si>
-  <si>
-    <t>Phillips</t>
-  </si>
-  <si>
-    <t>No. 2</t>
-  </si>
-  <si>
-    <t>Class 6h</t>
+    <t>System of Measurement</t>
+  </si>
+  <si>
+    <t>Class 6H</t>
+  </si>
+  <si>
+    <t>Thread</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Pitch</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Spacing</t>
+  </si>
+  <si>
+    <t>Fit</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>8 mm</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>5 mm</t>
+  </si>
+  <si>
+    <t>Insert Maximum Temperature</t>
+  </si>
+  <si>
+    <t>220° F</t>
+  </si>
+  <si>
+    <t>Specifications Met</t>
+  </si>
+  <si>
+    <t>DIN 985, ISO 10511</t>
+  </si>
+  <si>
+    <t>External Hex</t>
+  </si>
+  <si>
+    <t>Nut Type</t>
+  </si>
+  <si>
+    <t>Locknut, Hex</t>
+  </si>
+  <si>
+    <t>Hex Nut Profile</t>
+  </si>
+  <si>
+    <t>Locking Type</t>
+  </si>
+  <si>
+    <t>Nylon Insert</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,6 +416,24 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF777777"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -461,7 +461,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -478,12 +478,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCBCBCB"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCBCBCB"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -530,12 +548,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -545,11 +557,50 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2952,6 +3003,1494 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="653143" y="3701143"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1025" name="AutoShape 1" descr="click to learn more about Right Hand">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6E259B5-CAF9-0234-A08A-FE24A7708FC3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="2057400"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1026" name="AutoShape 2" descr="click to learn more about ">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D77067D-4D2E-4531-142D-0FBCF1EDDECB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="2447925"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1027" name="AutoShape 3" descr="click to learn more about M2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB5C04A0-18A3-4D69-C508-9DD3EB92817E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="2447925"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1028" name="AutoShape 4" descr="click to learn more about Metric">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E18422AF-C335-3AC8-FA35-D00E45E6A787}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="3152775"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1029" name="AutoShape 5" descr="click to learn more about ">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6053B308-34A2-2AAF-8A42-5E62CE8EF130}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="3543300"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1030" name="AutoShape 6" descr="click to learn more about Coarse">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DD06D87-606C-269C-AF6B-FEF4F1013E0A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="3543300"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1031" name="AutoShape 7" descr="click to learn more about Right Hand">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9D0E63C-BAE7-337C-A38A-4C8E9129AC0A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="2057400"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1032" name="AutoShape 8" descr="click to learn more about ">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A91C073-AC22-B3EE-CE88-838750F6E9E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="2447925"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1033" name="AutoShape 9" descr="click to learn more about M3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B360B3E-1D6C-5F07-D1DE-05515AB4FEFB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="2447925"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1034" name="AutoShape 10" descr="click to learn more about Metric">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DD3E74D-F931-A077-2AAD-9B84D2A0F3A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="3152775"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1035" name="AutoShape 11" descr="click to learn more about ">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{923947F4-6F36-11BB-EF21-7A1E503FDDBB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="3543300"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1036" name="AutoShape 12" descr="click to learn more about Coarse">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02A5C854-AE44-C891-8CB5-51FB8E69BFF2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="3543300"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1037" name="AutoShape 13" descr="click to learn more about Right Hand">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3A6F953-A1AA-1AD1-E4BF-B9ABEF2B47AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="2057400"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1038" name="AutoShape 14" descr="click to learn more about ">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0CB30C9-0C00-BD7A-8E18-C47A44834FA1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="2447925"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1039" name="AutoShape 15" descr="click to learn more about M5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6849FD6B-A019-3245-0B05-A7D45B203880}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="2447925"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1040" name="AutoShape 16" descr="click to learn more about Metric">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2940533F-C77C-9B38-E08B-06C746644AAA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="3152775"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1041" name="AutoShape 17" descr="click to learn more about ">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00354B9C-333E-64E4-E7F2-F117CC1AC4DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="3543300"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1042" name="AutoShape 18" descr="click to learn more about Coarse">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BEFEFC5-0BF4-B09B-A666-B2723B660A06}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="3543300"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1043" name="AutoShape 19" descr="click to learn more about Right Hand">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BF1F0FE-C733-7FF9-7E12-87994A2C6DE4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="2057400"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1044" name="AutoShape 20" descr="click to learn more about ">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A01C3616-CC76-DE82-C408-B9275E7542A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="2447925"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1045" name="AutoShape 21" descr="click to learn more about M6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3025995C-5384-689F-BA2C-D7FEF9B2765D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="2447925"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1046" name="AutoShape 22" descr="click to learn more about Metric">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{292A5C5D-9720-FB82-CE9D-DA0E5D51577B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="3152775"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1047" name="AutoShape 23" descr="click to learn more about ">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDA96635-25BE-2FCC-2C7F-4ADF3EDA446A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="3543300"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1048" name="AutoShape 24" descr="click to learn more about Coarse">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAE493FE-1AB3-A434-C437-D79301DE9414}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="3543300"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1049" name="AutoShape 25" descr="click to learn more about ">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{327D056C-CC1B-F080-A75A-02B95E449ECF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="381000"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1050" name="AutoShape 26" descr="click to learn more about M5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{884BBE77-C571-E799-358C-2E111751FC21}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1051" name="AutoShape 27" descr="click to learn more about Metric">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3C69E86-847D-9B5F-126D-FBC0348A2743}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="952500"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1052" name="AutoShape 28" descr="click to learn more about ">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9228DD98-57F7-F7B8-3013-8209E4F125CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="1333500"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1053" name="AutoShape 29" descr="click to learn more about Coarse">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D208DDD0-B92A-9F48-4B4C-730916E80C6A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="1333500"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1054" name="AutoShape 30" descr="click to learn more about Right Hand">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A23C23FB-E6A3-7931-C087-F814EE87705D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="1905000"/>
+          <a:ext cx="114300" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1055" name="AutoShape 31" descr="click to learn more about External Hex">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60BB796C-E87E-5FBA-F071-BDF1FEBB2075}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="3905250"/>
           <a:ext cx="114300" cy="114300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3278,13 +4817,13 @@
       <selection activeCell="C6" sqref="C6:C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="49.07421875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.765625" customWidth="1"/>
+    <col min="3" max="3" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>49</v>
       </c>
@@ -3296,7 +4835,7 @@
         <v>Category: Integrated Circuits (ICs)</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="12" t="s">
         <v>51</v>
@@ -3306,7 +4845,7 @@
         <v>: Logic - Shift Registers</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
@@ -3318,7 +4857,7 @@
         <v>Mfr: Texas Instruments</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>54</v>
       </c>
@@ -3330,8 +4869,8 @@
         <v>Series: 74HC</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
         <v>56</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -3342,8 +4881,8 @@
         <v>Package: Tape &amp; Reel (TR)</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6" s="16"/>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
       <c r="B6" s="2" t="s">
         <v>58</v>
       </c>
@@ -3352,8 +4891,8 @@
         <v>: Cut Tape (CT)</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7" s="16"/>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
       <c r="B7" s="2" t="s">
         <v>59</v>
       </c>
@@ -3362,7 +4901,7 @@
         <v>: Digi-Reel®</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>3</v>
       </c>
@@ -3374,7 +4913,7 @@
         <v>Product Status: Active</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>60</v>
       </c>
@@ -3386,7 +4925,7 @@
         <v>Logic Type: Shift Register</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>62</v>
       </c>
@@ -3398,7 +4937,7 @@
         <v>Output Type: Complementary</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>64</v>
       </c>
@@ -3410,7 +4949,7 @@
         <v>Number of Elements: 1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>65</v>
       </c>
@@ -3422,7 +4961,7 @@
         <v>Number of Bits per Element: 8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>66</v>
       </c>
@@ -3434,7 +4973,7 @@
         <v>Function: Parallel or Serial to Serial</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>68</v>
       </c>
@@ -3446,7 +4985,7 @@
         <v>Voltage - Supply: 2V ~ 6V</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -3458,7 +4997,7 @@
         <v>Operating Temperature: -40°C ~ 125°C</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>5</v>
       </c>
@@ -3470,7 +5009,7 @@
         <v>Mounting Type: Surface Mount</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
@@ -3482,7 +5021,7 @@
         <v>Package / Case: 16-TSSOP (0.173", 4.40mm Width)</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>2</v>
       </c>
@@ -3494,7 +5033,7 @@
         <v>Supplier Device Package: 16-TSSOP</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -3506,7 +5045,7 @@
         <v>Base Product Number: 74HC165</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.45" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>25</v>
       </c>
@@ -3518,7 +5057,7 @@
         <v>Product Type:: FFC &amp; FPC Connectors</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>28</v>
       </c>
@@ -3530,7 +5069,7 @@
         <v>Subcategory:: FFC &amp; FPC Connectors</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>9</v>
       </c>
@@ -3542,7 +5081,7 @@
         <v>Actuator Color: Black</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
@@ -3554,7 +5093,7 @@
         <v>Mating Cycles: 20</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
@@ -3589,9 +5128,9 @@
       <selection activeCell="C20" sqref="C1:C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
@@ -3603,7 +5142,7 @@
         <v>Manufacturer: Molex</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.45" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>31</v>
       </c>
@@ -3615,7 +5154,7 @@
         <v>Product Category: FFC / FPC Jumper Cables</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>33</v>
       </c>
@@ -3627,7 +5166,7 @@
         <v>RoHS:  Details</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.45" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>35</v>
       </c>
@@ -3639,7 +5178,7 @@
         <v>Number of Conductors: 40 Conductor</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
@@ -3651,7 +5190,7 @@
         <v>Pitch: 0.5 mm</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>37</v>
       </c>
@@ -3663,7 +5202,7 @@
         <v>Cable Length: 203 mm</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.45" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
@@ -3675,7 +5214,7 @@
         <v>Contact Location: Same Side Contacts</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>17</v>
       </c>
@@ -3687,7 +5226,7 @@
         <v>Current Rating: 500 mA</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>40</v>
       </c>
@@ -3699,7 +5238,7 @@
         <v>Voltage Rating: 600 VAC</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
@@ -3711,7 +5250,7 @@
         <v>Series: 15366</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>23</v>
       </c>
@@ -3723,7 +5262,7 @@
         <v>Packaging: Bulk</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>24</v>
       </c>
@@ -3735,7 +5274,7 @@
         <v>Brand: Molex</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
@@ -3747,7 +5286,7 @@
         <v>Contact Plating: Tin</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="23.15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" ht="33" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>22</v>
       </c>
@@ -3759,7 +5298,7 @@
         <v>Maximum Operating Temperature: + 105 C</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="23.15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" ht="33" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>20</v>
       </c>
@@ -3771,7 +5310,7 @@
         <v>Minimum Operating Temperature: - 40 C</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.45" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>25</v>
       </c>
@@ -3783,7 +5322,7 @@
         <v>Product Type: FFC / FPC Jumper Cables</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.45" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>27</v>
       </c>
@@ -3795,7 +5334,7 @@
         <v>Factory Pack Quantity: 20</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>28</v>
       </c>
@@ -3807,7 +5346,7 @@
         <v>Subcategory: Cable</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>45</v>
       </c>
@@ -3819,7 +5358,7 @@
         <v>Tradename: Premo-Flex</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>47</v>
       </c>
@@ -3831,7 +5370,7 @@
         <v>Part # Aliases: 153660439 0153660439</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>28</v>
       </c>
@@ -3843,7 +5382,7 @@
         <v>Subcategory: FFC &amp; FPC Connectors</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>9</v>
       </c>
@@ -3855,7 +5394,7 @@
         <v>Actuator Color Black</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
@@ -3867,7 +5406,7 @@
         <v>Mating Cycles: 20</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
@@ -3894,362 +5433,344 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32416015-4403-4A02-9DF3-D08E90EF15EE}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C23"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="27.61328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>102</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="B1" s="22"/>
       <c r="C1" t="str">
         <f t="shared" ref="C1:C37" si="0">CONCATENATE(A1,": ",B1)</f>
-        <v>Thread Size: M5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" s="21"/>
-      <c r="B2" s="19"/>
+        <v xml:space="preserve">Thread: </v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>79</v>
+      </c>
       <c r="C2" t="str">
         <f t="shared" si="0"/>
+        <v>Size: M5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
         <v xml:space="preserve">: </v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" s="20" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>Pitch: 0.8 mm</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>Type: Metric</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="31"/>
+      <c r="B6" s="32"/>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">: </v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>Spacing: Coarse</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="31"/>
+      <c r="B8" s="32"/>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">: </v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>Fit: Class 6H</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>Direction: Right Hand</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="33"/>
+      <c r="B11" s="27"/>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">: </v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>Width: 8 mm</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>Height: 5 mm</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>Insert Maximum Temperature: 220° F</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>Specifications Met: DIN 985, ISO 10511</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B16" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>Drive Style: External Hex</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="25"/>
+      <c r="B17" s="27"/>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">: </v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>Nut Type: Locknut, Hex</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>Hex Nut Profile: Standard</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="C3" t="str">
-        <f t="shared" si="0"/>
-        <v>Thread Pitch: 0.8 mm</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" s="20" t="s">
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>Locking Type: Nylon Insert</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="48" x14ac:dyDescent="0.25">
+      <c r="A21" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="C4" t="str">
-        <f t="shared" si="0"/>
-        <v>Length: 20 mm</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" t="str">
-        <f t="shared" si="0"/>
-        <v>Threading: Fully Threaded</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" t="str">
-        <f t="shared" si="0"/>
-        <v>Head Diameter: 9.2 mm</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" t="str">
-        <f t="shared" si="0"/>
-        <v>Head Height: 2.5 mm</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" t="str">
-        <f t="shared" si="0"/>
-        <v>Countersink Angle: 90°</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A9" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="C9" t="str">
-        <f t="shared" si="0"/>
-        <v>Drive Style: Phillips</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A10" s="21"/>
-      <c r="B10" s="19"/>
-      <c r="C10" t="str">
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>System of Measurement: Metric</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="19"/>
+      <c r="B22" s="16"/>
+      <c r="C22" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">: </v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A11" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="C11" t="str">
-        <f t="shared" si="0"/>
-        <v>Drive Size: No. 2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A12" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" t="str">
-        <f t="shared" si="0"/>
-        <v>Material: Zinc-Plated Steel</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" t="str">
-        <f t="shared" si="0"/>
-        <v>Hardness: Rockwell B71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A14" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" t="str">
-        <f t="shared" si="0"/>
-        <v>Tensile Strength: 60,000 psi</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A15" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="C15" t="str">
-        <f t="shared" si="0"/>
-        <v>Thread Type: Metric</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A16" s="21"/>
-      <c r="B16" s="19"/>
-      <c r="C16" t="str">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="18"/>
+      <c r="B23" s="17"/>
+      <c r="C23" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">: </v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A17" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="C17" t="str">
-        <f t="shared" si="0"/>
-        <v>Thread Spacing: Coarse</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A18" s="21"/>
-      <c r="B18" s="19"/>
-      <c r="C18" t="str">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="18"/>
+      <c r="B24" s="17"/>
+      <c r="C24" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">: </v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A19" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="C19" t="str">
-        <f t="shared" si="0"/>
-        <v>Thread Fit: Class 6h</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A20" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="C20" t="str">
-        <f t="shared" si="0"/>
-        <v>Thread Direction: Right Hand</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A21" s="21"/>
-      <c r="B21" s="19"/>
-      <c r="C21" t="str">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="19"/>
+      <c r="B25" s="16"/>
+      <c r="C25" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">: </v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A22" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="C22" t="str">
-        <f t="shared" si="0"/>
-        <v>Head Type: Flat</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A23" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="C23" t="str">
-        <f t="shared" si="0"/>
-        <v>Flat Head Profile: Standard</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A24" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="C24" t="str">
-        <f t="shared" si="0"/>
-        <v>Head Type: Flat</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A25" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="C25" t="str">
-        <f t="shared" si="0"/>
-        <v>Flat Head Profile: Standard</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C26" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">: </v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C27" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">: </v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C28" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">: </v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">: </v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C30" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">: </v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C31" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">: </v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C32" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">: </v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">: </v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">: </v>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">: </v>
       </c>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">: </v>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">: </v>
@@ -4257,19 +5778,20 @@
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="134" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4279,7 +5801,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>